<commit_message>
correção de erros na planilha
</commit_message>
<xml_diff>
--- a/excel/template.xlsx
+++ b/excel/template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC7A7FF4-74F1-4D2B-9C6F-30F8A2BE8CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF7130F0-866B-4B20-82B5-60171ECDA872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAPA" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="257">
   <si>
     <t>PLANILHA PARA SOLICITAÇÃO DE CANCELAMENTO DE CARTÕES</t>
-  </si>
-  <si>
-    <t>V-S2601</t>
   </si>
   <si>
     <t>Resumo da solicitação de cancelamento cartão:</t>
@@ -827,7 +824,7 @@
     <numFmt numFmtId="172" formatCode="_-&quot;R$ &quot;* #,##0.00_-;&quot;-R$ &quot;* #,##0.00_-;_-&quot;R$ &quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="173" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,7 +946,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1032,6 +1029,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF0070C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -1221,19 +1224,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1241,23 +1238,8 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1503,21 +1485,27 @@
     <xf numFmtId="172" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1539,14 +1527,24 @@
     <xf numFmtId="14" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="172" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1564,33 +1562,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1598,7 +1580,6 @@
   <dxfs count="13">
     <dxf>
       <font>
-        <strike/>
         <color rgb="FFFFFFFF"/>
       </font>
       <fill>
@@ -1686,6 +1667,7 @@
     </dxf>
     <dxf>
       <font>
+        <strike/>
         <color rgb="FFFFFFFF"/>
       </font>
       <fill>
@@ -1923,365 +1905,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:Q25"/>
+  <dimension ref="B5:M25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="2" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
     <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="15" width="3" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" customWidth="1"/>
-    <col min="17" max="17" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:17" ht="23.25" customHeight="1">
+    <row r="5" spans="2:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="98" t="s">
+      <c r="C5" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row r="6" spans="2:17">
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="99" t="s">
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="95"/>
+    </row>
+    <row r="7" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="D8" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="99"/>
-    </row>
-    <row r="7" spans="2:17" ht="13.5" customHeight="1">
-      <c r="B7" s="2"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row r="8" spans="2:17" ht="18.75" customHeight="1">
-      <c r="B8" s="2"/>
-      <c r="D8" s="100" t="s">
+      <c r="E8" s="97"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="100"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="101"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="5"/>
-      <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="2:17">
-      <c r="B9" s="2"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="123"/>
-      <c r="O9" s="4"/>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="B10" s="2"/>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="5"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="D11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="123"/>
-      <c r="L10" s="123"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="4"/>
-      <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="2:17">
-      <c r="B11" s="2"/>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="6"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
+      <c r="D12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="123"/>
-      <c r="O11" s="4"/>
-      <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="2:17">
-      <c r="B12" s="2"/>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="D13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="123"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="123"/>
-      <c r="O12" s="4"/>
-      <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="2:17">
-      <c r="B13" s="2"/>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="D14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="123"/>
-      <c r="O13" s="4"/>
-      <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="2:17">
-      <c r="B14" s="2"/>
-      <c r="D14" s="6" t="s">
+      <c r="E14" s="6"/>
+      <c r="G14" s="117"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="G15" s="117"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="D16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="123"/>
-      <c r="J14" s="123"/>
-      <c r="K14" s="123"/>
-      <c r="L14" s="123"/>
-      <c r="M14" s="123"/>
-      <c r="N14" s="123"/>
-      <c r="O14" s="4"/>
-      <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="2:17" ht="10.5" customHeight="1">
-      <c r="B15" s="2"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="123"/>
-      <c r="J15" s="123"/>
-      <c r="K15" s="123"/>
-      <c r="L15" s="123"/>
-      <c r="M15" s="123"/>
-      <c r="N15" s="123"/>
-      <c r="O15" s="4"/>
-      <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="2:17">
-      <c r="B16" s="2"/>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="6"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="D17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="123"/>
-      <c r="J16" s="123"/>
-      <c r="K16" s="123"/>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="4"/>
-      <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="2:17" ht="14.25" customHeight="1">
-      <c r="B17" s="2"/>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="E18" s="7"/>
+      <c r="G18" s="119"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="D19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="123"/>
-      <c r="J17" s="123"/>
-      <c r="K17" s="123"/>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="2:17" ht="10.5" customHeight="1">
-      <c r="B18" s="2"/>
-      <c r="E18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
-      <c r="K18" s="123"/>
-      <c r="L18" s="123"/>
-      <c r="M18" s="123"/>
-      <c r="N18" s="123"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="2:17">
-      <c r="B19" s="2"/>
-      <c r="D19" s="6" t="s">
+      <c r="E19" s="7"/>
+      <c r="G19" s="119"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="4"/>
-    </row>
-    <row r="20" spans="2:17">
-      <c r="B20" s="2"/>
-      <c r="D20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="13" t="str">
+      <c r="E20" s="7" t="str">
         <f>IF(TRANSACAO!D12="","",TRANSACAO!D12)</f>
         <v/>
       </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="2:17" ht="10.5" customHeight="1">
+      <c r="G20" s="120"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="4"/>
-    </row>
-    <row r="22" spans="2:17">
+      <c r="G21" s="120"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="D23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="2:17">
-      <c r="B23" s="2"/>
-      <c r="D23" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="I23" s="102"/>
-      <c r="J23" s="102"/>
-      <c r="K23" s="102"/>
-      <c r="L23" s="102"/>
-      <c r="M23" s="102"/>
-      <c r="N23" s="102"/>
-      <c r="O23" s="102"/>
-      <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="2:17" ht="7.5" customHeight="1">
+      <c r="E23" s="10"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
-      <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="2:17">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="O781qRP8dpUG3+nBUliA8wed4ZA4bEJg4V0o8mH6IQby6WKiB+VEeFzIBXufNz2STSPU6XgstxsnRFVbNyD/sw==" saltValue="p9yQxJXZkZCHuAp2BNkfLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="6">
-    <mergeCell ref="D5:N6"/>
-    <mergeCell ref="O6:Q6"/>
+  <mergeCells count="2">
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="H8:N8"/>
-    <mergeCell ref="I23:O23"/>
-    <mergeCell ref="H9:N18"/>
+    <mergeCell ref="C5:G6"/>
   </mergeCells>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2290,384 +2105,341 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S44"/>
+  <dimension ref="B1:S44"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" style="124" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="124" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="28" style="124" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="124" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="20" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="20" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="20" customWidth="1"/>
-    <col min="11" max="11" width="9" style="20" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="20" customWidth="1"/>
-    <col min="16" max="16" width="28" style="20" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" style="20" customWidth="1"/>
-    <col min="18" max="16384" width="10.140625" style="20"/>
+    <col min="1" max="1" width="3.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="13" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="13" customWidth="1"/>
+    <col min="11" max="11" width="9" style="13" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" style="13" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" style="13" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="28" style="13" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" style="13" customWidth="1"/>
+    <col min="18" max="16384" width="10.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="26.25" customHeight="1">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
+    <row r="1" spans="3:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="E2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="H2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="K2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="L2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="M2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="O2" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="P2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="21" t="s">
+    </row>
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" s="20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="82.5" customHeight="1">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-    </row>
-    <row r="7" spans="1:19" ht="111" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:19" hidden="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="23" t="str">
+      <c r="Q3" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="3:19" ht="82.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="3:19" ht="111" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="3:19" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="16" t="str">
         <f>"4" &amp; TEXT(INT(D8),"yymmdd")</f>
         <v>4000100</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="24" t="s">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C10" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="24" t="s">
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C11" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="24"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="121" t="s">
+      <c r="D11" s="91"/>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="121"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="24" t="s">
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C13" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="24" t="s">
+      <c r="D13" s="17"/>
+    </row>
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="24" t="s">
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C15" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="17"/>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C16" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="25" t="s">
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="25"/>
-    </row>
-    <row r="17" spans="3:4" s="20" customFormat="1">
-      <c r="C17" s="24" t="s">
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="3:4" s="20" customFormat="1">
-      <c r="C18" s="24" t="s">
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="19" spans="3:4" s="20" customFormat="1">
-      <c r="C19" s="24" t="s">
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="3:4" s="20" customFormat="1">
-      <c r="C20" s="24" t="s">
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="3:4" s="20" customFormat="1">
-      <c r="C21" s="24" t="s">
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="3:4" s="20" customFormat="1">
-      <c r="C22" s="24" t="s">
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="3:4" s="20" customFormat="1">
-      <c r="C23" s="24" t="s">
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="24"/>
-    </row>
-    <row r="24" spans="3:4" s="20" customFormat="1">
-      <c r="C24" s="22" t="s">
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="22"/>
-    </row>
-    <row r="25" spans="3:4" s="20" customFormat="1">
-      <c r="C25" s="24" t="s">
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="24"/>
-    </row>
-    <row r="26" spans="3:4" s="20" customFormat="1">
-      <c r="C26" s="24" t="s">
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="24"/>
-    </row>
-    <row r="27" spans="3:4" s="20" customFormat="1">
-      <c r="C27" s="24" t="s">
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="24"/>
-    </row>
-    <row r="28" spans="3:4" s="20" customFormat="1">
-      <c r="C28" s="24" t="s">
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="24"/>
-    </row>
-    <row r="29" spans="3:4" s="20" customFormat="1">
-      <c r="C29" s="24" t="s">
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="24"/>
-    </row>
-    <row r="30" spans="3:4" s="20" customFormat="1">
-      <c r="C30" s="24" t="s">
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="31" spans="3:4" s="20" customFormat="1">
-      <c r="C31" s="24" t="s">
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="24"/>
-    </row>
-    <row r="32" spans="3:4" s="20" customFormat="1">
-      <c r="C32" s="125" t="s">
+      <c r="D32" s="93"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="125"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="24"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="C34" s="122"/>
-      <c r="D34" s="122"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="C35" s="126"/>
-      <c r="D35" s="126"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="C36" s="126"/>
-      <c r="D36" s="126"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="C37" s="126"/>
-      <c r="D37" s="126"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="C38" s="126"/>
-      <c r="D38" s="126"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="C39" s="126"/>
-      <c r="D39" s="126"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="C40" s="126"/>
-      <c r="D40" s="126"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="C41" s="126"/>
-      <c r="D41" s="126"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="C42" s="126"/>
-      <c r="D42" s="126"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="C43" s="126"/>
-      <c r="D43" s="126"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="C44" s="127"/>
-      <c r="D44" s="127"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="92"/>
+      <c r="D34" s="92"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="94"/>
+      <c r="D39" s="94"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="42"/>
+      <c r="D44" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2683,525 +2455,525 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="15" style="26" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="26" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="26" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="38.7109375" style="26" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="26" customWidth="1"/>
-    <col min="12" max="12" width="39" style="26" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" style="26" customWidth="1"/>
-    <col min="14" max="14" width="39.5703125" style="26" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" style="26" customWidth="1"/>
-    <col min="16" max="16" width="34.140625" style="26" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" style="26" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" style="26" customWidth="1"/>
-    <col min="19" max="19" width="26.140625" style="26" customWidth="1"/>
-    <col min="20" max="20" width="19.7109375" style="26" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" style="26" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="26" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="9.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15" style="19" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="19" customWidth="1"/>
+    <col min="12" max="12" width="39" style="19" customWidth="1"/>
+    <col min="13" max="13" width="33.28515625" style="19" customWidth="1"/>
+    <col min="14" max="14" width="39.5703125" style="19" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" style="19" customWidth="1"/>
+    <col min="16" max="16" width="34.140625" style="19" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" style="19" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" style="19" customWidth="1"/>
+    <col min="19" max="19" width="26.140625" style="19" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" style="19" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="19" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="19" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21">
-      <c r="B2" s="103" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" s="98" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="98"/>
+      <c r="U2" s="98"/>
+    </row>
+    <row r="3" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-    </row>
-    <row r="3" spans="2:21" ht="30" customHeight="1">
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="H3" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="I3" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="J3" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="K3" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="L3" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="M3" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="27" t="s">
+      <c r="O3" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="O3" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="P3" s="30" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21">
-      <c r="B4" s="31" t="str">
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="str">
         <f>IF(CAPA!E10="","",CAPA!E10)</f>
         <v/>
       </c>
-      <c r="C4" s="32" t="str">
+      <c r="C4" s="25" t="str">
         <f>IF(CAPA!E11="","",CAPA!E11)</f>
         <v/>
       </c>
-      <c r="D4" s="32" t="str">
+      <c r="D4" s="25" t="str">
         <f>IF(CAPA!E12="","",CAPA!E12)</f>
         <v/>
       </c>
-      <c r="E4" s="32" t="str">
+      <c r="E4" s="25" t="str">
         <f>IF(CAPA!E13="","",CAPA!E13)</f>
         <v/>
       </c>
-      <c r="F4" s="32" t="str">
+      <c r="F4" s="25" t="str">
         <f>IF(CAPA!E16="","",CAPA!E16)</f>
         <v/>
       </c>
-      <c r="G4" s="32" t="str">
+      <c r="G4" s="25" t="str">
         <f>IF(CAPA!E17="","",CAPA!E17)</f>
         <v/>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="24">
         <f>D12</f>
         <v>0</v>
       </c>
-      <c r="I4" s="33">
+      <c r="I4" s="26">
         <f>TRANSACAO!J3</f>
         <v>0</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="26">
         <f>G12</f>
         <v>0</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="25">
         <f>H8</f>
         <v>0</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L4" s="27">
         <f>TRANSACAO!D24</f>
         <v>0</v>
       </c>
-      <c r="M4" s="32">
+      <c r="M4" s="25">
         <f>VALUE(TRANSACAO!D13)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="34">
+      <c r="N4" s="27">
         <f>I12</f>
         <v>0</v>
       </c>
-      <c r="O4" s="32" t="str">
+      <c r="O4" s="25" t="str">
         <f>TRANSACAO!P3</f>
         <v/>
       </c>
-      <c r="P4" s="35">
+      <c r="P4" s="28">
         <f>H12</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="26" t="s">
+      <c r="Q4" s="29"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="U4" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="U4" s="26" t="s">
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="99" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="2:21">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="Q5" s="36"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-    </row>
-    <row r="6" spans="2:21">
-      <c r="B6" s="104" t="s">
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="99"/>
+      <c r="N6" s="99"/>
+      <c r="O6" s="99"/>
+      <c r="P6" s="99"/>
+      <c r="Q6" s="99"/>
+    </row>
+    <row r="7" spans="2:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-      <c r="E6" s="104"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="104"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="104"/>
-      <c r="N6" s="104"/>
-      <c r="O6" s="104"/>
-      <c r="P6" s="104"/>
-      <c r="Q6" s="104"/>
-    </row>
-    <row r="7" spans="2:21" ht="30" customHeight="1">
-      <c r="B7" s="40" t="s">
+      <c r="E7" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="40" t="s">
+      <c r="G7" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="41" t="s">
+      <c r="H7" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="42" t="s">
+      <c r="L7" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="40" t="s">
+      <c r="N7" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="O7" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="O7" s="40" t="s">
+      <c r="P7" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="P7" s="40" t="s">
+      <c r="Q7" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="Q7" s="40" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21">
-      <c r="B8" s="32">
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="25">
         <f>CAPA!E12</f>
         <v>0</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="27">
         <f>CAPA!E22</f>
         <v>0</v>
       </c>
-      <c r="D8" s="32" t="str">
+      <c r="D8" s="25" t="str">
         <f>G4</f>
         <v/>
       </c>
-      <c r="E8" s="32" t="str">
+      <c r="E8" s="25" t="str">
         <f>F4</f>
         <v/>
       </c>
-      <c r="F8" s="32" t="str">
+      <c r="F8" s="25" t="str">
         <f>E4</f>
         <v/>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="27">
         <f>CAPA!E22</f>
         <v>0</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="27">
         <f>TRANSACAO!D26</f>
         <v>0</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="27">
         <f>TRANSACAO!D24</f>
         <v>0</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="27">
         <f>TRANSACAO!D13</f>
         <v>0</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="27">
         <f>J8</f>
         <v>0</v>
       </c>
-      <c r="L8" s="32" t="str">
+      <c r="L8" s="25" t="str">
         <f>O4</f>
         <v/>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="27">
         <f>CAPA!E10</f>
         <v>0</v>
       </c>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-    </row>
-    <row r="10" spans="2:21">
-      <c r="B10" s="43"/>
-    </row>
-    <row r="11" spans="2:21">
-      <c r="B11" s="44" t="s">
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="36"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="D11" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="E11" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="F11" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="G11" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="H11" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="44" t="s">
+      <c r="I11" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="J11" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="J11" s="44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21">
-      <c r="B12" s="38">
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="31">
         <f>CAPA!E14</f>
         <v>0</v>
       </c>
-      <c r="C12" s="45" t="str">
+      <c r="C12" s="38" t="str">
         <f>TRANSACAO!E8</f>
         <v>4000100</v>
       </c>
-      <c r="D12" s="46">
+      <c r="D12" s="39">
         <f>TRANSACAO!D8</f>
         <v>0</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="38">
         <f>TRANSACAO!D11</f>
         <v>0</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="39">
         <f>D12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="40">
         <f>IF(TRANSACAO!D15&lt;&gt;"",TRANSACAO!D15,TRANSACAO!J3)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="41">
         <f>CAPA!E23</f>
         <v>0</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="19">
         <f>TRANSACAO!D20</f>
         <v>0</v>
       </c>
-      <c r="J12" s="45" t="s">
+      <c r="J12" s="38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="N13" s="42"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="44"/>
+      <c r="N15" s="42"/>
+    </row>
+    <row r="16" spans="2:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="100" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="N13" s="49"/>
-    </row>
-    <row r="14" spans="2:21">
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="P14" s="50"/>
-    </row>
-    <row r="15" spans="2:21">
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="49"/>
-    </row>
-    <row r="16" spans="2:21" ht="33" customHeight="1">
-      <c r="B16" s="105" t="s">
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="106"/>
-      <c r="D16" s="107"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="49"/>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="52" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="108" t="str">
+      <c r="C17" s="103" t="str">
         <f>IFERROR(VLOOKUP(CAPA!E14,Planilha1!A:C,3,TRUE),"")</f>
         <v/>
       </c>
-      <c r="D17" s="108"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="49"/>
-    </row>
-    <row r="18" spans="2:14">
-      <c r="B18" s="52" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="109">
+      <c r="D17" s="103"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="104">
         <f>IFERROR(G12,"")</f>
         <v>0</v>
       </c>
-      <c r="D18" s="109"/>
-    </row>
-    <row r="19" spans="2:14">
-      <c r="B19" s="52" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="110" t="str">
+      <c r="D18" s="104"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="106" t="str">
         <f>IFERROR(#REF!,"")</f>
         <v/>
       </c>
-      <c r="D19" s="110"/>
-    </row>
-    <row r="20" spans="2:14">
-      <c r="B20" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="111">
+      <c r="D19" s="106"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="107">
         <f>H12</f>
         <v>0</v>
       </c>
-      <c r="D20" s="108"/>
-    </row>
-    <row r="21" spans="2:14">
-      <c r="B21" s="52" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="108">
+      <c r="D20" s="103"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="103">
         <f>K8</f>
         <v>0</v>
       </c>
-      <c r="D21" s="108"/>
-    </row>
-    <row r="22" spans="2:14">
-      <c r="B22" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="C22" s="112" t="e">
+      <c r="D21" s="103"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="105" t="e">
         <f>VLOOKUP(CAPA!E14,Planilha1!A:D,4,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D22" s="112"/>
-    </row>
-    <row r="23" spans="2:14">
-      <c r="B23" s="52" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="108">
+      <c r="D22" s="105"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="103">
         <f>E12</f>
         <v>0</v>
       </c>
-      <c r="D23" s="108"/>
-    </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="52" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="108">
+      <c r="D23" s="103"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="103">
         <f>H8</f>
         <v>0</v>
       </c>
-      <c r="D24" s="108"/>
-    </row>
-    <row r="25" spans="2:14">
-      <c r="B25" s="52" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="112">
+      <c r="D24" s="103"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="105">
         <f>CAPA!E12</f>
         <v>0</v>
       </c>
-      <c r="D25" s="108"/>
+      <c r="D25" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3218,20 +2990,20 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
   </mergeCells>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="expression" dxfId="12" priority="1">
+      <formula>NOT(ISERROR(SEARCH("VERDECARD",B16)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>NOT(ISERROR(SEARCH("BANRICOMPRAS",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:Q7">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>NOT(ISERROR(SEARCH("VERDECARD",B7)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>NOT(ISERROR(SEARCH("BANRICOMPRAS",B7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="10" priority="1">
-      <formula>NOT(ISERROR(SEARCH("VERDECARD",B16)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>NOT(ISERROR(SEARCH("BANRICOMPRAS",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3248,859 +3020,859 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="53" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>88</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1006957020</v>
       </c>
       <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="53">
+      <c r="D4" s="46">
         <v>41123700000300</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2778065800</v>
       </c>
       <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
         <v>100</v>
       </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="53">
+      <c r="D5" s="46">
         <v>41123700006900</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1006956740</v>
       </c>
       <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
         <v>102</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="53">
+      <c r="D6" s="46">
         <v>41123700000500</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2895942891</v>
       </c>
       <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="53">
+      <c r="D7" s="46">
         <v>41123700008500</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1006957003</v>
       </c>
       <c r="B8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" t="s">
         <v>106</v>
       </c>
-      <c r="C8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="53">
+      <c r="D8" s="46">
         <v>41123700002500</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1015704848</v>
       </c>
       <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="C9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="53">
+      <c r="D9" s="46">
         <v>41123700002300</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2778140896</v>
       </c>
       <c r="B10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" t="s">
         <v>110</v>
       </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" s="53">
+      <c r="D10" s="46">
         <v>41123700004600</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1014953569</v>
       </c>
       <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
         <v>112</v>
       </c>
-      <c r="C11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="53">
+      <c r="D11" s="46">
         <v>41123700001300</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1034211312</v>
       </c>
       <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
         <v>114</v>
       </c>
-      <c r="C12" t="s">
-        <v>115</v>
-      </c>
-      <c r="D12" s="53">
+      <c r="D12" s="46">
         <v>41123700004100</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1015704988</v>
       </c>
       <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
         <v>116</v>
       </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" s="53">
+      <c r="D13" s="46">
         <v>41123700002900</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1059465350</v>
       </c>
       <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
         <v>118</v>
       </c>
-      <c r="C14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="53">
+      <c r="D14" s="46">
         <v>41123700004000</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1006957046</v>
       </c>
       <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
         <v>120</v>
       </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="53">
+      <c r="D15" s="46">
         <v>41123700002100</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1006956937</v>
       </c>
       <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" t="s">
         <v>122</v>
       </c>
-      <c r="C16" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="53">
+      <c r="D16" s="46">
         <v>41123700002400</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1034211290</v>
       </c>
       <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" t="s">
         <v>124</v>
       </c>
-      <c r="C17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="53">
+      <c r="D17" s="46">
         <v>41123700004200</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1040073198</v>
       </c>
       <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
         <v>126</v>
       </c>
-      <c r="C18" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="53">
+      <c r="D18" s="46">
         <v>41123700003900</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1034211282</v>
       </c>
       <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" t="s">
         <v>128</v>
       </c>
-      <c r="C19" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="53">
+      <c r="D19" s="46">
         <v>41123700000400</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1006956929</v>
       </c>
       <c r="B20" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" t="s">
         <v>130</v>
       </c>
-      <c r="C20" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="53">
+      <c r="D20" s="46">
         <v>41123700001600</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1006956910</v>
       </c>
       <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21" t="s">
         <v>132</v>
       </c>
-      <c r="C21" t="s">
-        <v>133</v>
-      </c>
-      <c r="D21" s="53">
+      <c r="D21" s="46">
         <v>41123700002700</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1012740967</v>
       </c>
       <c r="B22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" t="s">
         <v>134</v>
       </c>
-      <c r="C22" t="s">
-        <v>135</v>
-      </c>
-      <c r="D22" s="53">
+      <c r="D22" s="46">
         <v>41123700003300</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1043852465</v>
       </c>
       <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" t="s">
         <v>136</v>
       </c>
-      <c r="C23" t="s">
-        <v>137</v>
-      </c>
-      <c r="D23" s="53">
+      <c r="D23" s="46">
         <v>41123700004300</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1013722784</v>
       </c>
       <c r="B24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" t="s">
         <v>138</v>
       </c>
-      <c r="C24" t="s">
-        <v>139</v>
-      </c>
-      <c r="D24" s="53">
+      <c r="D24" s="46">
         <v>41123700003500</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1020269011</v>
       </c>
       <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" t="s">
         <v>140</v>
       </c>
-      <c r="C25" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="53">
+      <c r="D25" s="46">
         <v>41123700003600</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1012456444</v>
       </c>
       <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" t="s">
         <v>142</v>
       </c>
-      <c r="C26" t="s">
-        <v>143</v>
-      </c>
-      <c r="D26" s="53">
+      <c r="D26" s="46">
         <v>41123700000800</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1067221201</v>
       </c>
       <c r="B27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" t="s">
         <v>144</v>
       </c>
-      <c r="C27" t="s">
-        <v>145</v>
-      </c>
-      <c r="D27" s="53">
+      <c r="D27" s="46">
         <v>41123700005400</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2760786956</v>
       </c>
       <c r="B28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" t="s">
         <v>146</v>
       </c>
-      <c r="C28" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="53">
+      <c r="D28" s="46">
         <v>41123700008600</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2896300737</v>
       </c>
       <c r="B29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" t="s">
         <v>148</v>
       </c>
-      <c r="C29" t="s">
-        <v>149</v>
-      </c>
-      <c r="D29" s="53">
+      <c r="D29" s="46">
         <v>41123700008400</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1006963038</v>
       </c>
       <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" t="s">
         <v>150</v>
       </c>
-      <c r="C30" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="53">
+      <c r="D30" s="46">
         <v>41123700001800</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1012411971</v>
       </c>
       <c r="B31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" t="s">
         <v>152</v>
       </c>
-      <c r="C31" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" s="53">
+      <c r="D31" s="46">
         <v>41123700003100</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2900505741</v>
       </c>
       <c r="B32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" t="s">
         <v>154</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="D32" s="53" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1006956899</v>
       </c>
       <c r="B33" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" t="s">
         <v>157</v>
       </c>
-      <c r="C33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="53">
+      <c r="D33" s="46">
         <v>41123700001700</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1096168615</v>
       </c>
       <c r="B34" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
         <v>159</v>
       </c>
-      <c r="C34" t="s">
-        <v>160</v>
-      </c>
-      <c r="D34" s="53">
+      <c r="D34" s="46">
         <v>41123700005000</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1096168607</v>
       </c>
       <c r="B35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
         <v>161</v>
       </c>
-      <c r="C35" t="s">
-        <v>162</v>
-      </c>
-      <c r="D35" s="53">
+      <c r="D35" s="46">
         <v>41123700004900</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1006963020</v>
       </c>
       <c r="B36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" t="s">
         <v>163</v>
       </c>
-      <c r="C36" t="s">
-        <v>164</v>
-      </c>
-      <c r="D36" s="53">
+      <c r="D36" s="46">
         <v>41123700002000</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1006956880</v>
       </c>
       <c r="B37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" t="s">
         <v>165</v>
       </c>
-      <c r="C37" t="s">
-        <v>166</v>
-      </c>
-      <c r="D37" s="53">
+      <c r="D37" s="46">
         <v>41123700001400</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1005526823</v>
       </c>
       <c r="B38" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" t="s">
         <v>167</v>
       </c>
-      <c r="C38" t="s">
-        <v>168</v>
-      </c>
-      <c r="D38" s="53">
+      <c r="D38" s="46">
         <v>41123700000200</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2897596974</v>
       </c>
       <c r="B39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" t="s">
         <v>169</v>
       </c>
-      <c r="C39" t="s">
-        <v>170</v>
-      </c>
-      <c r="D39" s="53">
+      <c r="D39" s="46">
         <v>41123700008100</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1014327900</v>
       </c>
       <c r="B40" t="s">
+        <v>170</v>
+      </c>
+      <c r="C40" t="s">
         <v>171</v>
       </c>
-      <c r="C40" t="s">
-        <v>172</v>
-      </c>
-      <c r="D40" s="53">
+      <c r="D40" s="46">
         <v>41123700001900</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1006956961</v>
       </c>
       <c r="B41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" t="s">
         <v>173</v>
       </c>
-      <c r="C41" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" s="53">
+      <c r="D41" s="46">
         <v>41123700001000</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1006957143</v>
       </c>
       <c r="B42" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" t="s">
         <v>175</v>
       </c>
-      <c r="C42" t="s">
-        <v>176</v>
-      </c>
-      <c r="D42" s="53">
+      <c r="D42" s="46">
         <v>41123700000900</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1006957135</v>
       </c>
       <c r="B43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" t="s">
         <v>177</v>
       </c>
-      <c r="C43" t="s">
-        <v>178</v>
-      </c>
-      <c r="D43" s="53">
+      <c r="D43" s="46">
         <v>41123700002600</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1012412013</v>
       </c>
       <c r="B44" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" t="s">
         <v>179</v>
       </c>
-      <c r="C44" t="s">
-        <v>180</v>
-      </c>
-      <c r="D44" s="53">
+      <c r="D44" s="46">
         <v>41123700002200</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1096168623</v>
       </c>
       <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" t="s">
         <v>181</v>
       </c>
-      <c r="C45" t="s">
-        <v>182</v>
-      </c>
-      <c r="D45" s="53">
+      <c r="D45" s="46">
         <v>41123700005100</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1006957119</v>
       </c>
       <c r="B46" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" t="s">
         <v>183</v>
       </c>
-      <c r="C46" t="s">
-        <v>184</v>
-      </c>
-      <c r="D46" s="53">
+      <c r="D46" s="46">
         <v>41123700001100</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1010678504</v>
       </c>
       <c r="B47" t="s">
+        <v>184</v>
+      </c>
+      <c r="C47" t="s">
         <v>185</v>
       </c>
-      <c r="C47" t="s">
-        <v>186</v>
-      </c>
-      <c r="D47" s="53">
+      <c r="D47" s="46">
         <v>41123700002800</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1006957100</v>
       </c>
       <c r="B48" t="s">
+        <v>186</v>
+      </c>
+      <c r="C48" t="s">
         <v>187</v>
       </c>
-      <c r="C48" t="s">
-        <v>188</v>
-      </c>
-      <c r="D48" s="53">
+      <c r="D48" s="46">
         <v>41123700001200</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1057448467</v>
       </c>
       <c r="B49" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" t="s">
         <v>189</v>
       </c>
-      <c r="C49" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" s="53">
+      <c r="D49" s="46">
         <v>41123700004500</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1096780124</v>
       </c>
       <c r="B50" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" t="s">
         <v>191</v>
       </c>
-      <c r="C50" t="s">
-        <v>192</v>
-      </c>
-      <c r="D50" s="53">
+      <c r="D50" s="46">
         <v>41123700006700</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1096168658</v>
       </c>
       <c r="B51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" t="s">
         <v>193</v>
       </c>
-      <c r="C51" t="s">
-        <v>194</v>
-      </c>
-      <c r="D51" s="53">
+      <c r="D51" s="46">
         <v>41123700006400</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2898427327</v>
       </c>
       <c r="B52" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" t="s">
         <v>195</v>
       </c>
-      <c r="C52" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1006956708</v>
       </c>
       <c r="B53" t="s">
+        <v>196</v>
+      </c>
+      <c r="C53" t="s">
         <v>197</v>
       </c>
-      <c r="C53" t="s">
-        <v>198</v>
-      </c>
-      <c r="D53" s="53">
+      <c r="D53" s="46">
         <v>41123700000100</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2897203069</v>
       </c>
       <c r="B54" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" t="s">
         <v>199</v>
       </c>
-      <c r="C54" t="s">
-        <v>200</v>
-      </c>
-      <c r="D54" s="53">
+      <c r="D54" s="46">
         <v>41123700009000</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2898296923</v>
       </c>
       <c r="B55" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" t="s">
         <v>201</v>
       </c>
-      <c r="C55" t="s">
-        <v>202</v>
-      </c>
-      <c r="D55" s="53">
+      <c r="D55" s="46">
         <v>41123700008300</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1014327862</v>
       </c>
       <c r="B56" t="s">
+        <v>202</v>
+      </c>
+      <c r="C56" t="s">
         <v>203</v>
       </c>
-      <c r="C56" t="s">
-        <v>204</v>
-      </c>
-      <c r="D56" s="53">
+      <c r="D56" s="46">
         <v>41123700003400</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1012195470</v>
       </c>
       <c r="B57" t="s">
+        <v>204</v>
+      </c>
+      <c r="C57" t="s">
         <v>205</v>
       </c>
-      <c r="C57" t="s">
-        <v>206</v>
-      </c>
-      <c r="D57" s="53">
+      <c r="D57" s="46">
         <v>41123700003000</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1027418330</v>
       </c>
       <c r="B58" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" t="s">
         <v>207</v>
       </c>
-      <c r="C58" t="s">
-        <v>208</v>
-      </c>
-      <c r="D58" s="53">
+      <c r="D58" s="46">
         <v>41123700003700</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1067221244</v>
       </c>
       <c r="B59" t="s">
+        <v>208</v>
+      </c>
+      <c r="C59" t="s">
         <v>209</v>
       </c>
-      <c r="C59" t="s">
-        <v>210</v>
-      </c>
-      <c r="D59" s="53">
+      <c r="D59" s="46">
         <v>41123700005500</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1006957097</v>
       </c>
       <c r="B60" t="s">
+        <v>210</v>
+      </c>
+      <c r="C60" t="s">
         <v>211</v>
       </c>
-      <c r="C60" t="s">
-        <v>212</v>
-      </c>
-      <c r="D60" s="53">
+      <c r="D60" s="46">
         <v>41123700000700</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1067221252</v>
       </c>
       <c r="B61" t="s">
+        <v>212</v>
+      </c>
+      <c r="C61" t="s">
         <v>213</v>
       </c>
-      <c r="C61" t="s">
-        <v>214</v>
-      </c>
-      <c r="D61" s="53">
+      <c r="D61" s="46">
         <v>41123700006300</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1045331691</v>
       </c>
       <c r="B62" t="s">
+        <v>214</v>
+      </c>
+      <c r="C62" t="s">
         <v>215</v>
       </c>
-      <c r="C62" t="s">
-        <v>216</v>
-      </c>
-      <c r="D62" s="53">
+      <c r="D62" s="46">
         <v>41123700003800</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1012369401</v>
       </c>
       <c r="B63" t="s">
+        <v>216</v>
+      </c>
+      <c r="C63" t="s">
         <v>217</v>
       </c>
-      <c r="C63" t="s">
-        <v>218</v>
-      </c>
-      <c r="D63" s="53">
+      <c r="D63" s="46">
         <v>41123700003200</v>
       </c>
     </row>
@@ -4117,14 +3889,14 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="11" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="30.5703125" customWidth="1"/>
@@ -4137,542 +3909,542 @@
     <col min="20" max="20" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1">
-      <c r="I1" s="54"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-    </row>
-    <row r="2" spans="1:17" ht="27" customHeight="1">
-      <c r="A2" s="56"/>
-      <c r="B2" s="113" t="s">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="47"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+    </row>
+    <row r="2" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="111" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="114" t="s">
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="51">
+        <v>1</v>
+      </c>
+      <c r="P2" s="51">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="58">
-        <v>1</v>
-      </c>
-      <c r="P2" s="58">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="58" t="s">
+    </row>
+    <row r="3" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52"/>
+      <c r="B3" s="53" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="45" customHeight="1">
-      <c r="A3" s="59"/>
-      <c r="B3" s="60" t="s">
+      <c r="C3" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="D3" s="53" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="E3" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="F3" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="G3" s="53" t="s">
         <v>226</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="H3" s="50"/>
+      <c r="I3" s="113" t="s">
         <v>227</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="115" t="s">
+      <c r="J3" s="113"/>
+      <c r="K3" s="113"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="51">
+        <v>2</v>
+      </c>
+      <c r="P3" s="51">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="J3" s="115"/>
-      <c r="K3" s="115"/>
-      <c r="L3" s="115"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="58">
-        <v>2</v>
-      </c>
-      <c r="P3" s="58">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="58" t="s">
+    </row>
+    <row r="4" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
+      <c r="B4" s="54" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="26.25" customHeight="1">
-      <c r="A4" s="56"/>
-      <c r="B4" s="61" t="s">
-        <v>230</v>
-      </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63">
+      <c r="C4" s="55"/>
+      <c r="D4" s="56">
         <f>ROUND(VALUE(C4)/E4,2)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="61">
+      <c r="E4" s="54">
         <v>30</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="G4" s="54" t="s">
         <v>231</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="H4" s="50"/>
+      <c r="I4" s="57" t="s">
         <v>232</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="64" t="s">
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="51">
+        <v>3</v>
+      </c>
+      <c r="P4" s="51">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="54" t="s">
         <v>233</v>
       </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="58">
-        <v>3</v>
-      </c>
-      <c r="P4" s="58">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="58" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="26.25" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="61" t="s">
-        <v>234</v>
-      </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63">
+      <c r="C5" s="55"/>
+      <c r="D5" s="56">
         <f>ROUND(VALUE(C5)/3,2)</f>
         <v>0</v>
       </c>
-      <c r="E5" s="61">
+      <c r="E5" s="54">
         <v>3</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="G5" s="54" t="s">
         <v>235</v>
       </c>
-      <c r="G5" s="61" t="s">
-        <v>236</v>
-      </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="66" t="e">
+      <c r="H5" s="50"/>
+      <c r="I5" s="59" t="e">
         <f>VLOOKUP(I4,#REF!,2,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="J5" s="67">
+      <c r="J5" s="60">
         <f>SUM(J13,G10)</f>
         <v>0</v>
       </c>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="58">
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="51">
         <v>6</v>
       </c>
-      <c r="P5" s="58">
+      <c r="P5" s="51">
         <v>6</v>
       </c>
-      <c r="Q5" s="58" t="s">
+      <c r="Q5" s="51" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="54" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="68"/>
-      <c r="B6" s="61" t="s">
-        <v>238</v>
-      </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63">
+      <c r="C6" s="55"/>
+      <c r="D6" s="56">
         <f>ROUND(VALUE(C6)/6,2)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="61">
+      <c r="E6" s="54">
         <v>6</v>
       </c>
-      <c r="F6" s="61" t="s">
+      <c r="F6" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="G6" s="54" t="s">
         <v>235</v>
       </c>
-      <c r="G6" s="61" t="s">
-        <v>236</v>
-      </c>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="58">
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="51">
         <v>7</v>
       </c>
-      <c r="P6" s="58">
+      <c r="P6" s="51">
         <v>12</v>
       </c>
-      <c r="Q6" s="58" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="68"/>
-      <c r="B7" s="61" t="s">
-        <v>239</v>
-      </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="63">
+      <c r="Q6" s="51" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="61"/>
+      <c r="B7" s="54" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="62"/>
+      <c r="D7" s="56">
         <f>ROUND(VALUE(C7)/12,2)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="61">
+      <c r="E7" s="54">
         <v>12</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="G7" s="54" t="s">
         <v>235</v>
       </c>
-      <c r="G7" s="61" t="s">
-        <v>236</v>
-      </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="70"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
-    </row>
-    <row r="9" spans="1:17" ht="45" customHeight="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="71" t="s">
-        <v>221</v>
-      </c>
-      <c r="C9" s="71" t="s">
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="63"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+    </row>
+    <row r="9" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="D9" s="71" t="s">
+      <c r="E9" s="64" t="s">
         <v>241</v>
       </c>
-      <c r="E9" s="71" t="s">
+      <c r="F9" s="64" t="s">
         <v>242</v>
       </c>
-      <c r="F9" s="71" t="s">
-        <v>243</v>
-      </c>
-      <c r="G9" s="71" t="str">
+      <c r="G9" s="64" t="str">
         <f>IF(G10&gt;=0, "Devolução ao Cliente","Gerar Nota de Crédito")</f>
         <v>Devolução ao Cliente</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-    </row>
-    <row r="10" spans="1:17" ht="16.350000000000001" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="76" t="str">
+      <c r="H9" s="50"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+    </row>
+    <row r="10" spans="1:17" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="69" t="str">
         <f>IF(D10="","",IFERROR(D10-C10,""))</f>
         <v/>
       </c>
-      <c r="F10" s="77" t="str">
+      <c r="F10" s="70" t="str">
         <f>IF(D10="","",IFERROR(D4*E10,""))</f>
         <v/>
       </c>
-      <c r="G10" s="77" t="str">
+      <c r="G10" s="70" t="str">
         <f>IF(D10="","",IFERROR(C4-F10,""))</f>
         <v/>
       </c>
-      <c r="H10" s="116"/>
-      <c r="I10" s="116"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="73"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="82" t="s">
-        <v>244</v>
-      </c>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-    </row>
-    <row r="12" spans="1:17" ht="45" customHeight="1">
-      <c r="A12" s="83" t="str">
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="75" t="s">
+        <v>243</v>
+      </c>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+    </row>
+    <row r="12" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="str">
         <f>IF(A13=1,"Trimestral",IF(A13=2,"Semestral",IF(A13=3,"Anual","")))</f>
         <v/>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="64" t="s">
+        <v>244</v>
+      </c>
+      <c r="C12" s="64" t="s">
         <v>245</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="D12" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="E12" s="64" t="s">
         <v>246</v>
       </c>
-      <c r="D12" s="84" t="s">
-        <v>241</v>
-      </c>
-      <c r="E12" s="71" t="s">
+      <c r="F12" s="64" t="s">
         <v>247</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="G12" s="64" t="s">
         <v>248</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="H12" s="64" t="s">
         <v>249</v>
       </c>
-      <c r="H12" s="71" t="s">
+      <c r="I12" s="64" t="s">
         <v>250</v>
       </c>
-      <c r="I12" s="71" t="s">
-        <v>251</v>
-      </c>
-      <c r="J12" s="71" t="str">
+      <c r="J12" s="64" t="str">
         <f>IF(IFERROR(IF(J13&lt;=0,"Valor a receber do cliente",IF(J13&gt;0,"Valor a devolver para o cliente")),"")=FALSE(),"",IFERROR(IF(J13&lt;=0,"Valor a receber do cliente",IF(J13&gt;0,"Valor a devolver para o cliente")),""))</f>
         <v>Valor a devolver para o cliente</v>
       </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="117" t="s">
-        <v>252</v>
-      </c>
-      <c r="M12" s="117"/>
-    </row>
-    <row r="13" spans="1:17" ht="16.350000000000001" customHeight="1">
-      <c r="A13" s="58" t="str">
+      <c r="K12" s="50"/>
+      <c r="L12" s="115" t="s">
+        <v>251</v>
+      </c>
+      <c r="M12" s="115"/>
+    </row>
+    <row r="13" spans="1:17" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="str">
         <f>IFERROR(IF(I5=2,1,IF(I5=3,2,IF(I5=4,3))),"")</f>
         <v/>
       </c>
-      <c r="B13" s="61" t="str">
+      <c r="B13" s="54" t="str">
         <f>A12</f>
         <v/>
       </c>
-      <c r="C13" s="75">
+      <c r="C13" s="68">
         <v>45870</v>
       </c>
-      <c r="D13" s="75">
+      <c r="D13" s="68">
         <v>46006</v>
       </c>
-      <c r="E13" s="76">
+      <c r="E13" s="69">
         <f>IFERROR(IF(AND(C13="", D13=""), "", SUM(DATEDIF(C13,D13,"M")+1)),"")</f>
         <v>5</v>
       </c>
-      <c r="F13" s="67" t="b">
+      <c r="F13" s="60" t="b">
         <f>IF(D13="","",IFERROR(IF(A12="TRIMESTRAL",C4-D5,IF(A12="SEMESTRAL",C4-D6,IF(A12="ANUAL",C4-D7))),""))</f>
         <v>0</v>
       </c>
-      <c r="G13" s="67">
+      <c r="G13" s="60">
         <f>IFERROR(F13*E13,"")</f>
         <v>0</v>
       </c>
-      <c r="H13" s="67" t="b">
+      <c r="H13" s="60" t="b">
         <f>IFERROR(IF(A12="TRIMESTRAL",D5*E13,IF(A12="SEMESTRAL",D6*E13,IF(A12="ANUAL",D7*E13))),"")</f>
         <v>0</v>
       </c>
-      <c r="I13" s="85">
+      <c r="I13" s="78">
         <f>IFERROR(IF(L13="Não", 0, G13+H13),"")</f>
         <v>0</v>
       </c>
-      <c r="J13" s="85" t="b">
+      <c r="J13" s="78" t="b">
         <f>IFERROR(IF(L13=2,IF(A12="trimestral",C5-H13,IF(A12="semestral",C6-H13,IF(A12="anual",C7-H13))),IF(A12="trimestral",C5-I13,IF(A12="semestral",C6-I13,IF(A12="anual",C7-I13)))),"")</f>
         <v>0</v>
       </c>
-      <c r="K13" s="57"/>
-      <c r="L13" s="118" t="str">
+      <c r="K13" s="50"/>
+      <c r="L13" s="108" t="str">
         <f>IFERROR(VLOOKUP(L11,#REF!,2,0),"")</f>
         <v/>
       </c>
-      <c r="M13" s="118"/>
-    </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1">
-      <c r="A14" s="70"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="86"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="70"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="119"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A16" s="70"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-    </row>
-    <row r="17" spans="1:14" ht="27" customHeight="1">
-      <c r="A17" s="65"/>
-      <c r="B17" s="120" t="s">
-        <v>253</v>
-      </c>
-      <c r="C17" s="120"/>
-      <c r="D17" s="120"/>
-      <c r="E17" s="120"/>
-      <c r="F17" s="120"/>
-      <c r="G17" s="120"/>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="88"/>
-      <c r="L17" s="88"/>
-    </row>
-    <row r="18" spans="1:14" ht="45" customHeight="1">
-      <c r="A18" s="83" t="e">
+      <c r="M13" s="108"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="63"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="79"/>
+      <c r="J14" s="109"/>
+      <c r="K14" s="109"/>
+      <c r="L14" s="109"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="63"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="109"/>
+      <c r="K15" s="109"/>
+      <c r="L15" s="109"/>
+    </row>
+    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="63"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+    </row>
+    <row r="17" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
+      <c r="B17" s="110" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" s="110"/>
+      <c r="D17" s="110"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="110"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="81"/>
+    </row>
+    <row r="18" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="76" t="e">
         <f>IF(A19=1,"trimestral",IF(A19=2,"semestral",IF(A19=3,"anual","")))</f>
         <v>#REF!</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="C18" s="53" t="s">
         <v>245</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="D18" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>253</v>
+      </c>
+      <c r="F18" s="53" t="s">
         <v>246</v>
       </c>
-      <c r="D18" s="60" t="s">
-        <v>241</v>
-      </c>
-      <c r="E18" s="60" t="s">
+      <c r="G18" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="F18" s="60" t="s">
-        <v>247</v>
-      </c>
-      <c r="G18" s="60" t="s">
+      <c r="H18" s="53" t="s">
         <v>255</v>
       </c>
-      <c r="H18" s="60" t="s">
+      <c r="I18" s="53" t="s">
         <v>256</v>
       </c>
-      <c r="I18" s="60" t="s">
-        <v>257</v>
-      </c>
-      <c r="K18" s="89"/>
-      <c r="L18" s="89"/>
-    </row>
-    <row r="19" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A19" s="90" t="e">
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+    </row>
+    <row r="19" spans="1:14" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="83" t="e">
         <f>VLOOKUP(A20,#REF!,3,0)</f>
         <v>#REF!</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="92"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="94" t="e">
+      <c r="B19" s="84"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="87" t="e">
         <f>IF(A19=1,VLOOKUP("Trimestral",B4:C7,2,0),IF(A19=2,VLOOKUP("Semestral",B4:C7,2,0),IF(A19=3,VLOOKUP("Anual",B4:C7,2,0))))</f>
         <v>#REF!</v>
       </c>
-      <c r="F19" s="95" t="str">
+      <c r="F19" s="88" t="str">
         <f>IFERROR(IF(AND(C19="", D19=""), "", SUM(DATEDIF(C19,D19,"M")+1)),"")</f>
         <v/>
       </c>
-      <c r="G19" s="67" t="str">
+      <c r="G19" s="60" t="str">
         <f>IFERROR(IF(A18="TRIMESTRAL",C4-D5,IF(A18="SEMESTRAL",C4-D6,IF(A18="ANUAL",C4-D7))),"")</f>
         <v/>
       </c>
-      <c r="H19" s="67" t="str">
+      <c r="H19" s="60" t="str">
         <f>IFERROR(G19*F19,"")</f>
         <v/>
       </c>
-      <c r="I19" s="67" t="str">
+      <c r="I19" s="60" t="str">
         <f>IFERROR(IF(A18="TRIMESTRAL",D5*F19,IF(A18="SEMESTRAL",D6*F19,IF(A18="ANUAL",D7*F19))),"")</f>
         <v/>
       </c>
-      <c r="K19" s="96"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="119"/>
-      <c r="N19" s="119"/>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="K19" s="89"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="109"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>233</v>
-      </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="D21" s="20"/>
+        <v>232</v>
+      </c>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D21" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -4686,43 +4458,41 @@
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="L12:M12"/>
   </mergeCells>
-  <conditionalFormatting sqref="L13">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>I5=5</formula>
+  <conditionalFormatting sqref="B9:G10 L17:N17 B17:I19 K18:N19">
+    <cfRule type="expression" dxfId="8" priority="7">
+      <formula>$I$5=4</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$I$5=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>$I$5=3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9 B9:G10 J9:J10 B11:J13 L12">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>$I$5=5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10 B12:N13 B14:H14 J14 M14:N15 B15:I15 B16:N16 L17:N17 B17:I19 K18:N19">
+    <cfRule type="expression" dxfId="4" priority="10">
+      <formula>$I$5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$I$5=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>$I$5=3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>$I$5=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9 B11:J13 J9:J10 L12 B9:G10">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$I$5=5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17:N17 K18:N19 B17:I19 B9:G10">
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>$I$5=4</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>$I$5=2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17:N17 K18:N19 B17:I19 B9:G10">
-    <cfRule type="expression" dxfId="1" priority="9">
-      <formula>$I$5=3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:N16 B14:H14 J14 L17:N17 K18:N19 B12:N13 B15:I15 M14:N15 B17:I19 H10">
-    <cfRule type="expression" dxfId="0" priority="10">
-      <formula>$I$5=1</formula>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>I5=5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.51180555555555596" right="0.51180555555555596" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>